<commit_message>
select_one_dropdown for location information with more if statements and (select dropdown) text added
</commit_message>
<xml_diff>
--- a/app/config/tables/checklist/forms/checklist/checklist.xlsx
+++ b/app/config/tables/checklist/forms/checklist/checklist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="324">
   <si>
     <t>comments</t>
   </si>
@@ -538,18 +538,6 @@
     <t>power_note</t>
   </si>
   <si>
-    <t>Mains Powered CCE?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDD CCE? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faulty component? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">User related failure (Improper usage)? </t>
-  </si>
-  <si>
     <t>mains_powered_cce</t>
   </si>
   <si>
@@ -725,6 +713,291 @@
   </si>
   <si>
     <t xml:space="preserve">selected(data('is_site_as_per_odp'), 'no') </t>
+  </si>
+  <si>
+    <t>selected(data('mains_powered_cce'), 'yes')</t>
+  </si>
+  <si>
+    <t>selected(data('sdd_cce'), 'yes')</t>
+  </si>
+  <si>
+    <t>selected(data('faulty_component'), 'yes')</t>
+  </si>
+  <si>
+    <t>selected(data('user_related_failure'), 'yes')</t>
+  </si>
+  <si>
+    <t>selected(data('user_guideline_on_cover'), 'yes')</t>
+  </si>
+  <si>
+    <t>selected(data('malfunction_template_supplied'), 'yes')</t>
+  </si>
+  <si>
+    <t>senegal</t>
+  </si>
+  <si>
+    <t>solomon_islands</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Uganda</t>
+  </si>
+  <si>
+    <t>uganda</t>
+  </si>
+  <si>
+    <t>central</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Eastern</t>
+  </si>
+  <si>
+    <t>Northern</t>
+  </si>
+  <si>
+    <t>Western</t>
+  </si>
+  <si>
+    <t>eastern</t>
+  </si>
+  <si>
+    <t>northern</t>
+  </si>
+  <si>
+    <t>western</t>
+  </si>
+  <si>
+    <t>Buikwe</t>
+  </si>
+  <si>
+    <t>Bukomansimbi</t>
+  </si>
+  <si>
+    <t>Butambala</t>
+  </si>
+  <si>
+    <t>Buvuma</t>
+  </si>
+  <si>
+    <t>Gomba</t>
+  </si>
+  <si>
+    <t>Kalangala</t>
+  </si>
+  <si>
+    <t>Kalungu</t>
+  </si>
+  <si>
+    <t>Kampala</t>
+  </si>
+  <si>
+    <t>Kayunga</t>
+  </si>
+  <si>
+    <t>Kiboga</t>
+  </si>
+  <si>
+    <t>Kyankwanzi</t>
+  </si>
+  <si>
+    <t>Luweero</t>
+  </si>
+  <si>
+    <t>Lwengo</t>
+  </si>
+  <si>
+    <t>Lyantonde</t>
+  </si>
+  <si>
+    <t>Masaka</t>
+  </si>
+  <si>
+    <t>Mityana</t>
+  </si>
+  <si>
+    <t>Mpigi</t>
+  </si>
+  <si>
+    <t>Mubende</t>
+  </si>
+  <si>
+    <t>Mukono</t>
+  </si>
+  <si>
+    <t>Nakaseke</t>
+  </si>
+  <si>
+    <t>Nakasongola</t>
+  </si>
+  <si>
+    <t>Rakai</t>
+  </si>
+  <si>
+    <t>Ssembabule</t>
+  </si>
+  <si>
+    <t>Wakiso</t>
+  </si>
+  <si>
+    <t>buikwe</t>
+  </si>
+  <si>
+    <t>bukomansimbi</t>
+  </si>
+  <si>
+    <t>butambala</t>
+  </si>
+  <si>
+    <t>buvuma</t>
+  </si>
+  <si>
+    <t>gomba</t>
+  </si>
+  <si>
+    <t>kalangala</t>
+  </si>
+  <si>
+    <t>kalungu</t>
+  </si>
+  <si>
+    <t>kampala</t>
+  </si>
+  <si>
+    <t>kayunga</t>
+  </si>
+  <si>
+    <t>kiboga</t>
+  </si>
+  <si>
+    <t>kyankwanzi</t>
+  </si>
+  <si>
+    <t>luweero</t>
+  </si>
+  <si>
+    <t>lwengo</t>
+  </si>
+  <si>
+    <t>lyantonde</t>
+  </si>
+  <si>
+    <t>masaka</t>
+  </si>
+  <si>
+    <t>mityana</t>
+  </si>
+  <si>
+    <t>mpigi</t>
+  </si>
+  <si>
+    <t>mubende</t>
+  </si>
+  <si>
+    <t>mukono</t>
+  </si>
+  <si>
+    <t>nakaseke</t>
+  </si>
+  <si>
+    <t>nakasongola</t>
+  </si>
+  <si>
+    <t>rakai</t>
+  </si>
+  <si>
+    <t>ssembabule</t>
+  </si>
+  <si>
+    <t>wakiso</t>
+  </si>
+  <si>
+    <t>region_list</t>
+  </si>
+  <si>
+    <t>district_list</t>
+  </si>
+  <si>
+    <t>country_list</t>
+  </si>
+  <si>
+    <t>locality_list</t>
+  </si>
+  <si>
+    <t>select_one_dropdown</t>
+  </si>
+  <si>
+    <t>Kawolo</t>
+  </si>
+  <si>
+    <t>Lugazi</t>
+  </si>
+  <si>
+    <t>Najja</t>
+  </si>
+  <si>
+    <t>Najjembe</t>
+  </si>
+  <si>
+    <t>Njeru</t>
+  </si>
+  <si>
+    <t>Ngogwe</t>
+  </si>
+  <si>
+    <t>Nyenga</t>
+  </si>
+  <si>
+    <t>Ssi-Bukunja</t>
+  </si>
+  <si>
+    <t>Wakisi</t>
+  </si>
+  <si>
+    <t>kawolo</t>
+  </si>
+  <si>
+    <t>lugazi</t>
+  </si>
+  <si>
+    <t>najja</t>
+  </si>
+  <si>
+    <t>najjembe</t>
+  </si>
+  <si>
+    <t>njeru</t>
+  </si>
+  <si>
+    <t>ngogwe</t>
+  </si>
+  <si>
+    <t>nyenga</t>
+  </si>
+  <si>
+    <t>nsi-Bukunja</t>
+  </si>
+  <si>
+    <t>wakisi</t>
+  </si>
+  <si>
+    <t>Mains Powered CCE? (select dropdown)</t>
+  </si>
+  <si>
+    <t>SDD CCE? (select dropdown)</t>
+  </si>
+  <si>
+    <t>Faulty component? (select dropdown)</t>
+  </si>
+  <si>
+    <t>User related failure (Improper usage)? (select dropdown)</t>
   </si>
 </sst>
 </file>
@@ -801,7 +1074,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -827,6 +1100,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text 2" xfId="2"/>
@@ -1110,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M168"/>
+  <dimension ref="A1:M180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B162" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="G131" sqref="G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,8 +1398,8 @@
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" style="12" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
@@ -1176,7 +1453,7 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="6"/>
@@ -1225,20 +1502,23 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>30</v>
+        <v>301</v>
+      </c>
+      <c r="E8" t="s">
+        <v>299</v>
       </c>
       <c r="F8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>37</v>
@@ -1246,7 +1526,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>30</v>
+        <v>301</v>
+      </c>
+      <c r="E9" t="s">
+        <v>297</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
@@ -1257,7 +1540,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>30</v>
+        <v>301</v>
+      </c>
+      <c r="E10" t="s">
+        <v>298</v>
       </c>
       <c r="F10" t="s">
         <v>42</v>
@@ -1268,7 +1554,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>30</v>
+        <v>301</v>
+      </c>
+      <c r="E11" t="s">
+        <v>300</v>
       </c>
       <c r="F11" t="s">
         <v>43</v>
@@ -1279,17 +1568,17 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F14" t="s">
         <v>49</v>
@@ -1344,12 +1633,12 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -1387,12 +1676,12 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1419,12 +1708,12 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
@@ -1465,10 +1754,10 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C33" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1484,7 +1773,7 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -1500,12 +1789,12 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="90" x14ac:dyDescent="0.25">
@@ -1574,12 +1863,12 @@
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1634,12 +1923,12 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1658,10 +1947,10 @@
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C53" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
@@ -1677,7 +1966,7 @@
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1696,10 +1985,10 @@
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C57" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
@@ -1715,17 +2004,17 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1752,12 +2041,12 @@
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1801,12 +2090,12 @@
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1850,12 +2139,12 @@
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1899,12 +2188,12 @@
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1923,10 +2212,10 @@
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C82" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1942,17 +2231,17 @@
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="87" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -2004,12 +2293,12 @@
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="93" spans="2:7" ht="60" x14ac:dyDescent="0.25">
@@ -2064,12 +2353,12 @@
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="99" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -2124,12 +2413,12 @@
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -2168,7 +2457,7 @@
         <v>145</v>
       </c>
       <c r="G107" s="12" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -2198,12 +2487,12 @@
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="112" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -2247,12 +2536,12 @@
     </row>
     <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="117" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -2285,10 +2574,10 @@
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C119" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="120" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -2315,17 +2604,17 @@
     </row>
     <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="125" spans="2:7" ht="75" x14ac:dyDescent="0.25">
@@ -2355,12 +2644,12 @@
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="129" spans="2:7" ht="60" x14ac:dyDescent="0.25">
@@ -2385,7 +2674,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
         <v>71</v>
       </c>
@@ -2393,46 +2682,34 @@
         <v>24</v>
       </c>
       <c r="F131" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G131" s="12" t="s">
-        <v>170</v>
+        <v>320</v>
       </c>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D132" t="s">
-        <v>78</v>
-      </c>
-      <c r="F132" t="s">
-        <v>175</v>
-      </c>
-      <c r="G132" s="12" t="s">
-        <v>80</v>
+      <c r="B132" t="s">
+        <v>219</v>
+      </c>
+      <c r="C132" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
-        <v>71</v>
-      </c>
-      <c r="E133" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="F133" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G133" s="12" t="s">
-        <v>171</v>
+        <v>80</v>
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D134" t="s">
-        <v>78</v>
-      </c>
-      <c r="F134" t="s">
-        <v>178</v>
-      </c>
-      <c r="G134" s="12" t="s">
-        <v>80</v>
+      <c r="B134" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
@@ -2443,196 +2720,172 @@
         <v>24</v>
       </c>
       <c r="F135" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G135" s="12" t="s">
-        <v>172</v>
+        <v>321</v>
       </c>
     </row>
     <row r="136" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D136" t="s">
+      <c r="B136" t="s">
+        <v>219</v>
+      </c>
+      <c r="C136" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
         <v>78</v>
       </c>
-      <c r="F136" t="s">
-        <v>179</v>
-      </c>
-      <c r="G136" s="12" t="s">
+      <c r="F137" t="s">
+        <v>174</v>
+      </c>
+      <c r="G137" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="137" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D137" t="s">
-        <v>71</v>
-      </c>
-      <c r="E137" t="s">
-        <v>24</v>
-      </c>
-      <c r="F137" t="s">
-        <v>180</v>
-      </c>
-      <c r="G137" s="12" t="s">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>71</v>
+      </c>
+      <c r="E139" t="s">
+        <v>24</v>
+      </c>
+      <c r="F139" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D138" t="s">
-        <v>78</v>
-      </c>
-      <c r="F138" t="s">
-        <v>181</v>
-      </c>
-      <c r="G138" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
-        <v>221</v>
+      <c r="G139" s="12" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="141" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+      <c r="C140" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
-        <v>71</v>
-      </c>
-      <c r="E141" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="F141" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="G141" s="12" t="s">
-        <v>182</v>
+        <v>80</v>
       </c>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>226</v>
-      </c>
-      <c r="C142" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
-        <v>30</v>
+        <v>71</v>
+      </c>
+      <c r="E143" t="s">
+        <v>24</v>
       </c>
       <c r="F143" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="G143" s="12" t="s">
-        <v>183</v>
+        <v>323</v>
       </c>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="145" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="C144" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D145" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="F145" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="G145" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="146" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D146" t="s">
-        <v>71</v>
-      </c>
-      <c r="E146" t="s">
-        <v>24</v>
-      </c>
-      <c r="F146" t="s">
-        <v>196</v>
-      </c>
-      <c r="G146" s="12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="147" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D147" t="s">
-        <v>93</v>
-      </c>
-      <c r="F147" t="s">
-        <v>197</v>
-      </c>
-      <c r="G147" s="12" t="s">
-        <v>186</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B149" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="150" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D150" t="s">
-        <v>29</v>
-      </c>
-      <c r="F150" t="s">
-        <v>198</v>
-      </c>
-      <c r="G150" s="12" t="s">
-        <v>187</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
+        <v>71</v>
+      </c>
+      <c r="E149" t="s">
+        <v>24</v>
+      </c>
+      <c r="F149" t="s">
+        <v>189</v>
+      </c>
+      <c r="G149" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>222</v>
+      </c>
+      <c r="C150" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
-        <v>71</v>
-      </c>
-      <c r="E151" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F151" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="G151" s="12" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D152" t="s">
-        <v>71</v>
-      </c>
-      <c r="E152" t="s">
-        <v>24</v>
-      </c>
-      <c r="F152" t="s">
-        <v>200</v>
-      </c>
-      <c r="G152" s="12" t="s">
-        <v>189</v>
+      <c r="B152" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="153" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
-        <v>71</v>
-      </c>
-      <c r="E153" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="F153" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="G153" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="154" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
         <v>71</v>
       </c>
@@ -2640,152 +2893,266 @@
         <v>24</v>
       </c>
       <c r="F154" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="G154" s="12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B155" t="s">
-        <v>221</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
+        <v>93</v>
+      </c>
+      <c r="F155" t="s">
+        <v>193</v>
+      </c>
+      <c r="G155" s="12" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="156" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="157" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D157" t="s">
-        <v>71</v>
-      </c>
-      <c r="E157" t="s">
-        <v>24</v>
-      </c>
-      <c r="F157" t="s">
-        <v>203</v>
-      </c>
-      <c r="G157" s="12" t="s">
-        <v>192</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="158" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D158" t="s">
-        <v>71</v>
-      </c>
-      <c r="E158" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F158" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="G158" s="12" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
     </row>
     <row r="159" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D159" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+      <c r="E159" t="s">
+        <v>24</v>
       </c>
       <c r="F159" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="G159" s="12" t="s">
-        <v>80</v>
+        <v>184</v>
       </c>
     </row>
     <row r="160" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B161" t="s">
-        <v>220</v>
+      <c r="D160" t="s">
+        <v>71</v>
+      </c>
+      <c r="E160" t="s">
+        <v>24</v>
+      </c>
+      <c r="F160" t="s">
+        <v>196</v>
+      </c>
+      <c r="G160" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
+        <v>71</v>
+      </c>
+      <c r="E161" t="s">
+        <v>24</v>
+      </c>
+      <c r="F161" t="s">
+        <v>197</v>
+      </c>
+      <c r="G161" s="12" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="162" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
-        <v>29</v>
+        <v>71</v>
+      </c>
+      <c r="E162" t="s">
+        <v>24</v>
       </c>
       <c r="F162" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="G162" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D165" t="s">
+        <v>71</v>
+      </c>
+      <c r="E165" t="s">
+        <v>24</v>
+      </c>
+      <c r="F165" t="s">
+        <v>199</v>
+      </c>
+      <c r="G165" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D166" t="s">
+        <v>71</v>
+      </c>
+      <c r="E166" t="s">
+        <v>24</v>
+      </c>
+      <c r="F166" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D163" t="s">
-        <v>71</v>
-      </c>
-      <c r="E163" t="s">
-        <v>24</v>
-      </c>
-      <c r="F163" t="s">
-        <v>212</v>
-      </c>
-      <c r="G163" s="12" t="s">
+      <c r="G166" s="12" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D164" t="s">
-        <v>71</v>
-      </c>
-      <c r="E164" t="s">
-        <v>24</v>
-      </c>
-      <c r="F164" t="s">
-        <v>213</v>
-      </c>
-      <c r="G164" s="12" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="165" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D165" t="s">
-        <v>71</v>
-      </c>
-      <c r="E165" t="s">
-        <v>24</v>
-      </c>
-      <c r="F165" t="s">
-        <v>214</v>
-      </c>
-      <c r="G165" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D166" t="s">
-        <v>78</v>
-      </c>
-      <c r="F166" t="s">
-        <v>215</v>
-      </c>
-      <c r="G166" s="12" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="167" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="168" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+      <c r="C167" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
-        <v>71</v>
-      </c>
-      <c r="E168" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="F168" t="s">
+        <v>206</v>
+      </c>
+      <c r="G168" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
         <v>217</v>
       </c>
-      <c r="G168" s="12" t="s">
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D172" t="s">
+        <v>29</v>
+      </c>
+      <c r="F172" t="s">
         <v>207</v>
+      </c>
+      <c r="G172" s="12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D173" t="s">
+        <v>71</v>
+      </c>
+      <c r="E173" t="s">
+        <v>24</v>
+      </c>
+      <c r="F173" t="s">
+        <v>208</v>
+      </c>
+      <c r="G173" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D174" t="s">
+        <v>71</v>
+      </c>
+      <c r="E174" t="s">
+        <v>24</v>
+      </c>
+      <c r="F174" t="s">
+        <v>209</v>
+      </c>
+      <c r="G174" s="12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D175" t="s">
+        <v>71</v>
+      </c>
+      <c r="E175" t="s">
+        <v>24</v>
+      </c>
+      <c r="F175" t="s">
+        <v>210</v>
+      </c>
+      <c r="G175" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>222</v>
+      </c>
+      <c r="C176" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D177" t="s">
+        <v>78</v>
+      </c>
+      <c r="F177" t="s">
+        <v>211</v>
+      </c>
+      <c r="G177" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D180" t="s">
+        <v>71</v>
+      </c>
+      <c r="E180" t="s">
+        <v>24</v>
+      </c>
+      <c r="F180" t="s">
+        <v>213</v>
+      </c>
+      <c r="G180" s="12" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2796,10 +3163,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2809,7 +3176,7 @@
     <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>22</v>
       </c>
@@ -2820,7 +3187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
@@ -2831,7 +3198,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>24</v>
       </c>
@@ -2842,35 +3209,485 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B14" t="s">
+        <v>273</v>
+      </c>
+      <c r="C14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" t="s">
+        <v>274</v>
+      </c>
+      <c r="C15" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B16" t="s">
+        <v>275</v>
+      </c>
+      <c r="C16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B17" t="s">
+        <v>276</v>
+      </c>
+      <c r="C17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C18" t="s">
+        <v>253</v>
+      </c>
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C19" t="s">
+        <v>254</v>
+      </c>
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B20" t="s">
+        <v>279</v>
+      </c>
+      <c r="C20" t="s">
+        <v>255</v>
+      </c>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B21" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B22" t="s">
+        <v>281</v>
+      </c>
+      <c r="C22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" s="13"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B23" t="s">
+        <v>282</v>
+      </c>
+      <c r="C23" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B24" t="s">
+        <v>283</v>
+      </c>
+      <c r="C24" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B25" t="s">
+        <v>284</v>
+      </c>
+      <c r="C25" t="s">
+        <v>260</v>
+      </c>
+      <c r="D25" s="13"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B26" t="s">
+        <v>285</v>
+      </c>
+      <c r="C26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B27" t="s">
+        <v>286</v>
+      </c>
+      <c r="C27" t="s">
+        <v>262</v>
+      </c>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B28" t="s">
+        <v>287</v>
+      </c>
+      <c r="C28" t="s">
+        <v>263</v>
+      </c>
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B29" t="s">
+        <v>288</v>
+      </c>
+      <c r="C29" t="s">
+        <v>264</v>
+      </c>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B30" t="s">
+        <v>289</v>
+      </c>
+      <c r="C30" t="s">
+        <v>265</v>
+      </c>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B31" t="s">
+        <v>290</v>
+      </c>
+      <c r="C31" t="s">
+        <v>266</v>
+      </c>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B32" t="s">
+        <v>291</v>
+      </c>
+      <c r="C32" t="s">
+        <v>267</v>
+      </c>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B33" t="s">
+        <v>292</v>
+      </c>
+      <c r="C33" t="s">
+        <v>268</v>
+      </c>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B34" t="s">
+        <v>293</v>
+      </c>
+      <c r="C34" t="s">
+        <v>269</v>
+      </c>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B35" t="s">
+        <v>294</v>
+      </c>
+      <c r="C35" t="s">
+        <v>270</v>
+      </c>
+      <c r="D35" s="13"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B36" t="s">
+        <v>295</v>
+      </c>
+      <c r="C36" t="s">
+        <v>271</v>
+      </c>
+      <c r="D36" s="13"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B37" t="s">
+        <v>296</v>
+      </c>
+      <c r="C37" t="s">
+        <v>272</v>
+      </c>
+      <c r="D37" s="13"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>310</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>